<commit_message>
Mon Jan 16 21:24:15 CST 2023
</commit_message>
<xml_diff>
--- a/计划/2023学习计划.xlsx
+++ b/计划/2023学习计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13100" activeTab="3"/>
+    <workbookView windowHeight="16700" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="13">
   <si>
     <t>早餐</t>
   </si>
@@ -105,13 +105,74 @@
   </si>
   <si>
     <r>
+      <t>1音频/1视频/10技术书/1习题</t>
+    </r>
+    <r>
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">10技术书
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1音频/1视频/10技术书/1习题</t>
+    </r>
+  </si>
+  <si>
+    <t>跑步</t>
+  </si>
+  <si>
+    <r>
+      <t>1音频/1视频/10技术书/1习题</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -901,7 +962,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -933,6 +994,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1767,7 +1831,7 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
+    <sheetView topLeftCell="A26" workbookViewId="0">
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
@@ -1842,25 +1906,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="12" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1952,25 +2016,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="5" t="s">
+      <c r="B13" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="C13" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="D13" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="E13" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="F13" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="G13" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="12" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1980,7 +2044,9 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -2050,25 +2116,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="G20" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="H20" s="5" t="s">
+      <c r="H20" s="12" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2148,25 +2214,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="E27" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="F27" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="G27" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="H27" s="12" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2222,13 +2288,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="12" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2275,8 +2341,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -2350,26 +2416,26 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>9</v>
+      <c r="B5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -2461,25 +2527,25 @@
         <v>3</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -2559,25 +2625,25 @@
         <v>3</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -2657,25 +2723,25 @@
         <v>3</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H27" s="10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -2731,13 +2797,13 @@
         <v>3</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -2783,8 +2849,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -2859,25 +2925,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -2969,25 +3035,25 @@
         <v>3</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3067,25 +3133,25 @@
         <v>3</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3165,10 +3231,10 @@
         <v>3</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Sun Jan 29 21:06:09 CST 2023
</commit_message>
<xml_diff>
--- a/计划/2023学习计划.xlsx
+++ b/计划/2023学习计划.xlsx
@@ -4,20 +4,22 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16700" activeTab="3"/>
+    <workbookView windowHeight="16700" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
     <sheet name="01" sheetId="2" r:id="rId2"/>
     <sheet name="02" sheetId="3" r:id="rId3"/>
     <sheet name="03" sheetId="4" r:id="rId4"/>
+    <sheet name="04" sheetId="5" r:id="rId5"/>
+    <sheet name="05" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="21">
   <si>
     <t>早餐</t>
   </si>
@@ -162,6 +164,24 @@
     <t>跑步</t>
   </si>
   <si>
+    <t>胸</t>
+  </si>
+  <si>
+    <t>背，跑</t>
+  </si>
+  <si>
+    <t>休息</t>
+  </si>
+  <si>
+    <t>肩</t>
+  </si>
+  <si>
+    <t>腿</t>
+  </si>
+  <si>
+    <t>休</t>
+  </si>
+  <si>
     <r>
       <t>1音频/1视频/10技术书/1习题</t>
     </r>
@@ -195,6 +215,12 @@
       <t xml:space="preserve">
 1音频/1视频/10技术书/1习题</t>
     </r>
+  </si>
+  <si>
+    <t>背</t>
+  </si>
+  <si>
+    <t>跑</t>
   </si>
   <si>
     <r>
@@ -962,7 +988,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1001,6 +1027,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1831,6 +1860,1092 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="18.75" style="1" customWidth="1"/>
+    <col min="2" max="8" width="25.5625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" s="1" customFormat="1" ht="89" customHeight="1" spans="1:8">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3">
+        <v>9</v>
+      </c>
+      <c r="D9" s="3">
+        <v>10</v>
+      </c>
+      <c r="E9" s="3">
+        <v>11</v>
+      </c>
+      <c r="F9" s="3">
+        <v>12</v>
+      </c>
+      <c r="G9" s="3">
+        <v>13</v>
+      </c>
+      <c r="H9" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" s="1" customFormat="1" ht="162" customHeight="1" spans="1:8">
+      <c r="A13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A16" s="2"/>
+      <c r="B16" s="3">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3">
+        <v>16</v>
+      </c>
+      <c r="D16" s="3">
+        <v>17</v>
+      </c>
+      <c r="E16" s="3">
+        <v>18</v>
+      </c>
+      <c r="F16" s="3">
+        <v>19</v>
+      </c>
+      <c r="G16" s="3">
+        <v>20</v>
+      </c>
+      <c r="H16" s="3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A18" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A19" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" s="1" customFormat="1" ht="118" customHeight="1" spans="1:8">
+      <c r="A20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="23" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A23" s="2"/>
+      <c r="B23" s="3">
+        <v>22</v>
+      </c>
+      <c r="C23" s="3">
+        <v>23</v>
+      </c>
+      <c r="D23" s="6">
+        <v>24</v>
+      </c>
+      <c r="E23" s="6">
+        <v>25</v>
+      </c>
+      <c r="F23" s="6">
+        <v>26</v>
+      </c>
+      <c r="G23" s="6">
+        <v>27</v>
+      </c>
+      <c r="H23" s="6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A25" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A26" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" s="1" customFormat="1" ht="119" customHeight="1" spans="1:8">
+      <c r="A27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A28" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A30" s="2"/>
+      <c r="B30" s="6">
+        <v>29</v>
+      </c>
+      <c r="C30" s="6">
+        <v>30</v>
+      </c>
+      <c r="D30" s="6">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A31" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A32" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A33" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" s="1" customFormat="1" ht="134" customHeight="1" spans="1:4">
+      <c r="A34" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A35" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A37" s="7"/>
+      <c r="B37" s="8"/>
+    </row>
+    <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A38" s="8"/>
+      <c r="B38" s="7"/>
+    </row>
+    <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A39" s="8"/>
+      <c r="B39" s="7"/>
+    </row>
+    <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A40" s="8"/>
+      <c r="B40" s="7"/>
+    </row>
+    <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
+      <c r="A41" s="8"/>
+      <c r="B41" s="9"/>
+    </row>
+    <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A42" s="8"/>
+      <c r="B42" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28:H28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="18.75" style="1" customWidth="1"/>
+    <col min="2" max="8" width="25.5625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" s="1" customFormat="1" ht="89" customHeight="1" spans="1:8">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3">
+        <v>9</v>
+      </c>
+      <c r="D9" s="3">
+        <v>10</v>
+      </c>
+      <c r="E9" s="3">
+        <v>11</v>
+      </c>
+      <c r="F9" s="3">
+        <v>12</v>
+      </c>
+      <c r="G9" s="3">
+        <v>13</v>
+      </c>
+      <c r="H9" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" s="1" customFormat="1" ht="162" customHeight="1" spans="1:8">
+      <c r="A13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A16" s="2"/>
+      <c r="B16" s="3">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3">
+        <v>16</v>
+      </c>
+      <c r="D16" s="3">
+        <v>17</v>
+      </c>
+      <c r="E16" s="3">
+        <v>18</v>
+      </c>
+      <c r="F16" s="3">
+        <v>19</v>
+      </c>
+      <c r="G16" s="3">
+        <v>20</v>
+      </c>
+      <c r="H16" s="3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A18" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A19" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" s="1" customFormat="1" ht="118" customHeight="1" spans="1:8">
+      <c r="A20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A23" s="2"/>
+      <c r="B23" s="3">
+        <v>22</v>
+      </c>
+      <c r="C23" s="3">
+        <v>23</v>
+      </c>
+      <c r="D23" s="6">
+        <v>24</v>
+      </c>
+      <c r="E23" s="6">
+        <v>25</v>
+      </c>
+      <c r="F23" s="6">
+        <v>26</v>
+      </c>
+      <c r="G23" s="6">
+        <v>27</v>
+      </c>
+      <c r="H23" s="6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A25" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A26" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" s="1" customFormat="1" ht="119" customHeight="1" spans="1:8">
+      <c r="A27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A28" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A30" s="2"/>
+      <c r="B30" s="6">
+        <v>29</v>
+      </c>
+      <c r="C30" s="6">
+        <v>30</v>
+      </c>
+      <c r="D30" s="6">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A31" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A32" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A33" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" s="1" customFormat="1" ht="134" customHeight="1" spans="1:4">
+      <c r="A34" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A35" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A37" s="7"/>
+      <c r="B37" s="8"/>
+    </row>
+    <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A38" s="8"/>
+      <c r="B38" s="7"/>
+    </row>
+    <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A39" s="8"/>
+      <c r="B39" s="7"/>
+    </row>
+    <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A40" s="8"/>
+      <c r="B40" s="7"/>
+    </row>
+    <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
+      <c r="A41" s="8"/>
+      <c r="B41" s="9"/>
+    </row>
+    <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A42" s="8"/>
+      <c r="B42" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H42"/>
+  <sheetViews>
     <sheetView topLeftCell="A26" workbookViewId="0">
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
@@ -1906,26 +3021,26 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>7</v>
+      <c r="B5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -2016,26 +3131,26 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="H13" s="12" t="s">
-        <v>8</v>
+      <c r="B13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -2044,9 +3159,7 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -2116,26 +3229,26 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="H20" s="12" t="s">
-        <v>8</v>
+      <c r="B20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -2214,26 +3327,26 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="H27" s="12" t="s">
-        <v>8</v>
+      <c r="B27" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -2288,14 +3401,14 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>8</v>
+      <c r="B34" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -2336,13 +3449,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34:D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -2416,26 +3529,26 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>11</v>
+      <c r="B5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -2526,26 +3639,26 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="10" t="s">
-        <v>11</v>
+      <c r="B13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -2624,26 +3737,26 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H20" s="10" t="s">
-        <v>11</v>
+      <c r="B20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -2722,26 +3835,26 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G27" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H27" s="10" t="s">
-        <v>11</v>
+      <c r="B27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -2796,14 +3909,14 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>11</v>
+      <c r="B34" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -2844,13 +3957,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34:D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -2925,25 +4038,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -3035,25 +4148,25 @@
         <v>3</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3133,25 +4246,25 @@
         <v>3</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3231,10 +4344,10 @@
         <v>3</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Wed Feb  8 17:44:37 CST 2023
</commit_message>
<xml_diff>
--- a/计划/2023学习计划.xlsx
+++ b/计划/2023学习计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16700" activeTab="2"/>
+    <workbookView windowHeight="13100" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="19">
   <si>
     <t>早餐</t>
   </si>
@@ -106,61 +106,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>1音频/1视频/10技术书/1习题</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>1音频/1视频/10技术书/1习题</t>
-    </r>
-  </si>
-  <si>
     <t>跑步</t>
   </si>
   <si>
@@ -183,6 +128,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>1音频/1视频/10技术书/1习题</t>
     </r>
     <r>
@@ -227,45 +179,10 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">1音频/1视频/10技术书/1习题
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
         <rFont val="Calibri"/>
         <charset val="134"/>
+        <scheme val="minor"/>
       </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体-简"/>
-        <charset val="134"/>
-      </rPr>
-      <t>非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/1视频/10技术书/1习题</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">1音频/1视频/10技术书/1习题
 </t>
     </r>
@@ -298,10 +215,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -333,32 +250,8 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -373,6 +266,21 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -380,11 +288,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -396,13 +304,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -411,45 +312,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -464,6 +328,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -471,7 +350,45 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -538,7 +455,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -550,37 +581,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -592,31 +617,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -629,90 +630,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -741,15 +658,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -761,6 +669,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -790,6 +707,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -806,6 +738,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -814,177 +755,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1022,14 +939,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1352,7 +1269,7 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="D28" workbookViewId="0">
       <selection activeCell="B34" sqref="B34:D34"/>
     </sheetView>
   </sheetViews>
@@ -1860,8 +1777,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -1935,25 +1852,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="11" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2045,26 +1962,26 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="H13" s="12" t="s">
-        <v>8</v>
+      <c r="B13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -2074,7 +1991,7 @@
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -2145,26 +2062,26 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="H20" s="12" t="s">
-        <v>8</v>
+      <c r="B20" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -2243,26 +2160,26 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="H27" s="12" t="s">
-        <v>8</v>
+      <c r="B27" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -2273,14 +2190,14 @@
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
-      <c r="F28" s="13" t="s">
+      <c r="F28" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G28" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G28" s="13" t="s">
+      <c r="H28" s="12" t="s">
         <v>11</v>
-      </c>
-      <c r="H28" s="13" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -2323,28 +2240,28 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>8</v>
+      <c r="B34" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A35" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="D35" s="12" t="s">
         <v>14</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
@@ -2382,8 +2299,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28:H28"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -2458,25 +2375,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -2495,26 +2412,26 @@
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="B7" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="2" t="s">
+      <c r="E7" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -2582,25 +2499,25 @@
         <v>3</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -2608,25 +2525,25 @@
         <v>6</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="E14" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -2693,26 +2610,26 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>16</v>
+      <c r="B20" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -2720,25 +2637,25 @@
         <v>6</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="E21" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="H21" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="23" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -2805,26 +2722,26 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G27" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="H27" s="10" t="s">
-        <v>19</v>
+      <c r="B27" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -2832,25 +2749,25 @@
         <v>6</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="E28" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="H28" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -2893,14 +2810,14 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>19</v>
+      <c r="B34" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -3022,25 +2939,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -3132,25 +3049,25 @@
         <v>3</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3230,25 +3147,25 @@
         <v>3</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3328,25 +3245,25 @@
         <v>3</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3402,13 +3319,13 @@
         <v>3</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -3454,8 +3371,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34:D34"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -3530,25 +3447,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -3640,7 +3557,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Thu Feb  9 00:19:06 CST 2023
</commit_message>
<xml_diff>
--- a/计划/2023学习计划.xlsx
+++ b/计划/2023学习计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="13100" activeTab="4"/>
+    <workbookView windowHeight="16700" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -2299,8 +2299,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:E13"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -2418,7 +2418,7 @@
       <c r="C7" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="12" t="s">
@@ -2427,10 +2427,10 @@
       <c r="F7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="12" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2510,13 +2510,13 @@
       <c r="E13" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="H13" s="11" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2610,25 +2610,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="E20" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F20" s="13" t="s">
+      <c r="F20" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G20" s="13" t="s">
+      <c r="G20" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H20" s="13" t="s">
+      <c r="H20" s="11" t="s">
         <v>15</v>
       </c>
     </row>
@@ -3371,8 +3371,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -3560,13 +3560,13 @@
         <v>18</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Sun Feb 26 10:18:26 CST 2023
</commit_message>
<xml_diff>
--- a/计划/2023学习计划.xlsx
+++ b/计划/2023学习计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16700" activeTab="4"/>
+    <workbookView windowHeight="16700" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="03" sheetId="4" r:id="rId4"/>
     <sheet name="04" sheetId="5" r:id="rId5"/>
     <sheet name="05" sheetId="6" r:id="rId6"/>
+    <sheet name="06" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="19">
   <si>
     <t>早餐</t>
   </si>
@@ -127,13 +128,20 @@
     <t>休</t>
   </si>
   <si>
+    <t>背</t>
+  </si>
+  <si>
+    <t>跑</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <strike/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <charset val="134"/>
+        <scheme val="minor"/>
       </rPr>
       <t>1音频/1视频/10技术书/1习题</t>
     </r>
@@ -141,8 +149,9 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <charset val="134"/>
+        <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
 </t>
@@ -152,8 +161,9 @@
         <strike/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <charset val="134"/>
+        <scheme val="minor"/>
       </rPr>
       <t>20非技术书</t>
     </r>
@@ -161,18 +171,13 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <charset val="134"/>
+        <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
 1音频/1视频/10技术书/1习题</t>
     </r>
-  </si>
-  <si>
-    <t>背</t>
-  </si>
-  <si>
-    <t>跑</t>
   </si>
   <si>
     <r>
@@ -215,8 +220,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
@@ -250,6 +255,98 @@
       <charset val="134"/>
     </font>
     <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -259,7 +356,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -273,38 +370,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -321,22 +386,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -349,56 +399,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -449,55 +454,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -509,31 +490,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -551,7 +514,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -563,7 +538,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -575,13 +568,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -593,43 +628,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -658,6 +663,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -677,7 +691,37 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -685,8 +729,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -706,45 +750,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -760,148 +765,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -942,11 +947,11 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -2190,13 +2195,13 @@
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
-      <c r="F28" s="12" t="s">
+      <c r="F28" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G28" s="12" t="s">
+      <c r="G28" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H28" s="12" t="s">
+      <c r="H28" s="13" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2254,13 +2259,13 @@
       <c r="A35" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C35" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D35" s="12" t="s">
+      <c r="D35" s="13" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2299,8 +2304,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28:C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -2390,10 +2395,10 @@
         <v>7</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -2412,25 +2417,25 @@
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="13" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2499,51 +2504,41 @@
         <v>3</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A14" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>14</v>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="13" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -2611,51 +2606,45 @@
         <v>3</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="2" t="s">
+      <c r="B21" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="2" t="s">
+      <c r="C21" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H21" s="2" t="s">
-        <v>14</v>
+      <c r="H21" s="13" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="23" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -2722,40 +2711,40 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F27" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G27" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H27" s="13" t="s">
-        <v>15</v>
+      <c r="B27" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A28" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>14</v>
@@ -2810,14 +2799,14 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>15</v>
+      <c r="B34" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -2863,8 +2852,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -2938,26 +2927,26 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>18</v>
+      <c r="B5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -3048,26 +3037,26 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>18</v>
+      <c r="B13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3146,26 +3135,26 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>18</v>
+      <c r="B20" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3244,26 +3233,26 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>18</v>
+      <c r="B27" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3318,14 +3307,14 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>18</v>
+      <c r="B34" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -3371,8 +3360,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -3569,13 +3558,13 @@
         <v>18</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3655,25 +3644,25 @@
         <v>3</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3753,25 +3742,25 @@
         <v>3</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3827,7 +3816,7 @@
         <v>3</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>4</v>
@@ -3870,6 +3859,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -4380,4 +4370,512 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H42"/>
+  <sheetViews>
+    <sheetView topLeftCell="D28" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34:D34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="18.75" style="1" customWidth="1"/>
+    <col min="2" max="8" width="25.5625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" s="1" customFormat="1" ht="89" customHeight="1" spans="1:8">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3">
+        <v>9</v>
+      </c>
+      <c r="D9" s="3">
+        <v>10</v>
+      </c>
+      <c r="E9" s="3">
+        <v>11</v>
+      </c>
+      <c r="F9" s="3">
+        <v>12</v>
+      </c>
+      <c r="G9" s="3">
+        <v>13</v>
+      </c>
+      <c r="H9" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" s="1" customFormat="1" ht="162" customHeight="1" spans="1:8">
+      <c r="A13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A16" s="2"/>
+      <c r="B16" s="3">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3">
+        <v>16</v>
+      </c>
+      <c r="D16" s="3">
+        <v>17</v>
+      </c>
+      <c r="E16" s="3">
+        <v>18</v>
+      </c>
+      <c r="F16" s="3">
+        <v>19</v>
+      </c>
+      <c r="G16" s="3">
+        <v>20</v>
+      </c>
+      <c r="H16" s="3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A18" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A19" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" s="1" customFormat="1" ht="118" customHeight="1" spans="1:8">
+      <c r="A20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="23" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A23" s="2"/>
+      <c r="B23" s="3">
+        <v>22</v>
+      </c>
+      <c r="C23" s="3">
+        <v>23</v>
+      </c>
+      <c r="D23" s="6">
+        <v>24</v>
+      </c>
+      <c r="E23" s="6">
+        <v>25</v>
+      </c>
+      <c r="F23" s="6">
+        <v>26</v>
+      </c>
+      <c r="G23" s="6">
+        <v>27</v>
+      </c>
+      <c r="H23" s="6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A25" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A26" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" s="1" customFormat="1" ht="119" customHeight="1" spans="1:8">
+      <c r="A27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A28" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A30" s="2"/>
+      <c r="B30" s="6">
+        <v>29</v>
+      </c>
+      <c r="C30" s="6">
+        <v>30</v>
+      </c>
+      <c r="D30" s="6">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A31" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A32" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A33" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" s="1" customFormat="1" ht="134" customHeight="1" spans="1:4">
+      <c r="A34" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A35" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A37" s="7"/>
+      <c r="B37" s="8"/>
+    </row>
+    <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A38" s="8"/>
+      <c r="B38" s="7"/>
+    </row>
+    <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A39" s="8"/>
+      <c r="B39" s="7"/>
+    </row>
+    <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A40" s="8"/>
+      <c r="B40" s="7"/>
+    </row>
+    <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
+      <c r="A41" s="8"/>
+      <c r="B41" s="9"/>
+    </row>
+    <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A42" s="8"/>
+      <c r="B42" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Mon Mar 20 14:35:07 CST 2023
</commit_message>
<xml_diff>
--- a/计划/2023学习计划.xlsx
+++ b/计划/2023学习计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16700" activeTab="5"/>
+    <workbookView windowHeight="16700" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="19">
   <si>
     <t>早餐</t>
   </si>
@@ -179,34 +179,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">1音频/1视频/10技术书/1习题
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>20非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/1视频/10技术书/1习题</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
@@ -277,16 +249,16 @@
       <strike/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <strike/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -936,7 +908,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -970,13 +942,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3915,25 +3890,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="11" t="s">
+      <c r="B5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="12" t="s">
         <v>7</v>
       </c>
     </row>
@@ -4025,25 +4000,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="H13" s="11" t="s">
+      <c r="B13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="12" t="s">
         <v>7</v>
       </c>
     </row>
@@ -4125,25 +4100,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="H20" s="11" t="s">
+      <c r="B20" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20" s="12" t="s">
         <v>7</v>
       </c>
     </row>
@@ -4223,25 +4198,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="H27" s="11" t="s">
+      <c r="B27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27" s="12" t="s">
         <v>7</v>
       </c>
     </row>
@@ -4303,13 +4278,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D34" s="11" t="s">
+      <c r="B34" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="12" t="s">
         <v>7</v>
       </c>
     </row>
@@ -4437,25 +4412,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="11" t="s">
+      <c r="B5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="12" t="s">
         <v>7</v>
       </c>
     </row>
@@ -4561,25 +4536,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="H13" s="11" t="s">
+      <c r="B13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="12" t="s">
         <v>7</v>
       </c>
     </row>
@@ -4663,25 +4638,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="H20" s="11" t="s">
+      <c r="B20" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20" s="12" t="s">
         <v>7</v>
       </c>
     </row>
@@ -4769,25 +4744,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="H27" s="11" t="s">
+      <c r="B27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27" s="12" t="s">
         <v>7</v>
       </c>
     </row>
@@ -4852,8 +4827,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:E14"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -4927,25 +4902,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="11" t="s">
+      <c r="B5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="12" t="s">
         <v>7</v>
       </c>
     </row>
@@ -5051,25 +5026,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="H13" s="11" t="s">
+      <c r="B13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="12" t="s">
         <v>7</v>
       </c>
     </row>
@@ -5089,13 +5064,13 @@
       <c r="E14" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="13" t="s">
         <v>14</v>
       </c>
     </row>
@@ -5163,25 +5138,547 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="H20" s="11" t="s">
+      <c r="B20" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A23" s="2"/>
+      <c r="B23" s="3">
+        <v>22</v>
+      </c>
+      <c r="C23" s="3">
+        <v>23</v>
+      </c>
+      <c r="D23" s="6">
+        <v>24</v>
+      </c>
+      <c r="E23" s="6">
+        <v>25</v>
+      </c>
+      <c r="F23" s="6">
+        <v>26</v>
+      </c>
+      <c r="G23" s="6">
+        <v>27</v>
+      </c>
+      <c r="H23" s="6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A25" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A26" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" s="1" customFormat="1" ht="119" customHeight="1" spans="1:8">
+      <c r="A27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A28" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A30" s="2"/>
+      <c r="B30" s="6">
+        <v>29</v>
+      </c>
+      <c r="C30" s="6">
+        <v>30</v>
+      </c>
+      <c r="D30" s="6">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A31" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A32" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A33" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" s="1" customFormat="1" ht="134" customHeight="1" spans="1:4">
+      <c r="A34" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A35" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A37" s="7"/>
+      <c r="B37" s="8"/>
+    </row>
+    <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A38" s="8"/>
+      <c r="B38" s="7"/>
+    </row>
+    <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A39" s="8"/>
+      <c r="B39" s="7"/>
+    </row>
+    <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A40" s="8"/>
+      <c r="B40" s="7"/>
+    </row>
+    <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
+      <c r="A41" s="8"/>
+      <c r="B41" s="9"/>
+    </row>
+    <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A42" s="8"/>
+      <c r="B42" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H42"/>
+  <sheetViews>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="18.75" style="1" customWidth="1"/>
+    <col min="2" max="8" width="25.5625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" s="1" customFormat="1" ht="89" customHeight="1" spans="1:8">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3">
+        <v>9</v>
+      </c>
+      <c r="D9" s="3">
+        <v>10</v>
+      </c>
+      <c r="E9" s="3">
+        <v>11</v>
+      </c>
+      <c r="F9" s="3">
+        <v>12</v>
+      </c>
+      <c r="G9" s="3">
+        <v>13</v>
+      </c>
+      <c r="H9" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" s="1" customFormat="1" ht="162" customHeight="1" spans="1:8">
+      <c r="A13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A16" s="2"/>
+      <c r="B16" s="3">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3">
+        <v>16</v>
+      </c>
+      <c r="D16" s="3">
+        <v>17</v>
+      </c>
+      <c r="E16" s="3">
+        <v>18</v>
+      </c>
+      <c r="F16" s="3">
+        <v>19</v>
+      </c>
+      <c r="G16" s="3">
+        <v>20</v>
+      </c>
+      <c r="H16" s="3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A18" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A19" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" s="1" customFormat="1" ht="118" customHeight="1" spans="1:8">
+      <c r="A20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20" s="12" t="s">
         <v>7</v>
       </c>
     </row>
@@ -5261,25 +5758,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="H27" s="11" t="s">
+      <c r="B27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27" s="12" t="s">
         <v>7</v>
       </c>
     </row>
@@ -5335,13 +5832,522 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D34" s="11" t="s">
+      <c r="B34" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A35" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A37" s="7"/>
+      <c r="B37" s="8"/>
+    </row>
+    <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A38" s="8"/>
+      <c r="B38" s="7"/>
+    </row>
+    <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A39" s="8"/>
+      <c r="B39" s="7"/>
+    </row>
+    <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A40" s="8"/>
+      <c r="B40" s="7"/>
+    </row>
+    <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
+      <c r="A41" s="8"/>
+      <c r="B41" s="9"/>
+    </row>
+    <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A42" s="8"/>
+      <c r="B42" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H42"/>
+  <sheetViews>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="18.75" style="1" customWidth="1"/>
+    <col min="2" max="8" width="25.5625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" s="1" customFormat="1" ht="89" customHeight="1" spans="1:8">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3">
+        <v>9</v>
+      </c>
+      <c r="D9" s="3">
+        <v>10</v>
+      </c>
+      <c r="E9" s="3">
+        <v>11</v>
+      </c>
+      <c r="F9" s="3">
+        <v>12</v>
+      </c>
+      <c r="G9" s="3">
+        <v>13</v>
+      </c>
+      <c r="H9" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" s="1" customFormat="1" ht="162" customHeight="1" spans="1:8">
+      <c r="A13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A16" s="2"/>
+      <c r="B16" s="3">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3">
+        <v>16</v>
+      </c>
+      <c r="D16" s="3">
+        <v>17</v>
+      </c>
+      <c r="E16" s="3">
+        <v>18</v>
+      </c>
+      <c r="F16" s="3">
+        <v>19</v>
+      </c>
+      <c r="G16" s="3">
+        <v>20</v>
+      </c>
+      <c r="H16" s="3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A18" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A19" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" s="1" customFormat="1" ht="118" customHeight="1" spans="1:8">
+      <c r="A20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="23" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A23" s="2"/>
+      <c r="B23" s="3">
+        <v>22</v>
+      </c>
+      <c r="C23" s="3">
+        <v>23</v>
+      </c>
+      <c r="D23" s="6">
+        <v>24</v>
+      </c>
+      <c r="E23" s="6">
+        <v>25</v>
+      </c>
+      <c r="F23" s="6">
+        <v>26</v>
+      </c>
+      <c r="G23" s="6">
+        <v>27</v>
+      </c>
+      <c r="H23" s="6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A25" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A26" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" s="1" customFormat="1" ht="119" customHeight="1" spans="1:8">
+      <c r="A27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A28" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A30" s="2"/>
+      <c r="B30" s="6">
+        <v>29</v>
+      </c>
+      <c r="C30" s="6">
+        <v>30</v>
+      </c>
+      <c r="D30" s="6">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A31" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A32" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A33" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" s="1" customFormat="1" ht="134" customHeight="1" spans="1:4">
+      <c r="A34" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="12" t="s">
         <v>7</v>
       </c>
     </row>
@@ -5383,7 +6389,515 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H42"/>
+  <sheetViews>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="18.75" style="1" customWidth="1"/>
+    <col min="2" max="8" width="25.5625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" s="1" customFormat="1" ht="89" customHeight="1" spans="1:8">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3">
+        <v>9</v>
+      </c>
+      <c r="D9" s="3">
+        <v>10</v>
+      </c>
+      <c r="E9" s="3">
+        <v>11</v>
+      </c>
+      <c r="F9" s="3">
+        <v>12</v>
+      </c>
+      <c r="G9" s="3">
+        <v>13</v>
+      </c>
+      <c r="H9" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" s="1" customFormat="1" ht="162" customHeight="1" spans="1:8">
+      <c r="A13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A16" s="2"/>
+      <c r="B16" s="3">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3">
+        <v>16</v>
+      </c>
+      <c r="D16" s="3">
+        <v>17</v>
+      </c>
+      <c r="E16" s="3">
+        <v>18</v>
+      </c>
+      <c r="F16" s="3">
+        <v>19</v>
+      </c>
+      <c r="G16" s="3">
+        <v>20</v>
+      </c>
+      <c r="H16" s="3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A18" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A19" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" s="1" customFormat="1" ht="118" customHeight="1" spans="1:8">
+      <c r="A20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="23" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A23" s="2"/>
+      <c r="B23" s="3">
+        <v>22</v>
+      </c>
+      <c r="C23" s="3">
+        <v>23</v>
+      </c>
+      <c r="D23" s="6">
+        <v>24</v>
+      </c>
+      <c r="E23" s="6">
+        <v>25</v>
+      </c>
+      <c r="F23" s="6">
+        <v>26</v>
+      </c>
+      <c r="G23" s="6">
+        <v>27</v>
+      </c>
+      <c r="H23" s="6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A25" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A26" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" s="1" customFormat="1" ht="119" customHeight="1" spans="1:8">
+      <c r="A27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A28" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A30" s="2"/>
+      <c r="B30" s="6">
+        <v>29</v>
+      </c>
+      <c r="C30" s="6">
+        <v>30</v>
+      </c>
+      <c r="D30" s="6">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A31" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A32" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A33" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" s="1" customFormat="1" ht="134" customHeight="1" spans="1:4">
+      <c r="A34" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A35" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A37" s="7"/>
+      <c r="B37" s="8"/>
+    </row>
+    <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A38" s="8"/>
+      <c r="B38" s="7"/>
+    </row>
+    <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A39" s="8"/>
+      <c r="B39" s="7"/>
+    </row>
+    <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A40" s="8"/>
+      <c r="B40" s="7"/>
+    </row>
+    <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
+      <c r="A41" s="8"/>
+      <c r="B41" s="9"/>
+    </row>
+    <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A42" s="8"/>
+      <c r="B42" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:H42"/>
@@ -5463,26 +6977,26 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>7</v>
+      <c r="B5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -5573,26 +7087,26 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>7</v>
+      <c r="B13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5671,26 +7185,26 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>7</v>
+      <c r="B20" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5769,26 +7283,26 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="H27" s="11" t="s">
-        <v>7</v>
+      <c r="B27" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5843,14 +7357,14 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>7</v>
+      <c r="B34" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -5887,18 +7401,17 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -5972,26 +7485,26 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>7</v>
+      <c r="B5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -6082,26 +7595,26 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>7</v>
+      <c r="B13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -6180,26 +7693,26 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H20" s="12" t="s">
-        <v>17</v>
+      <c r="B20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -6278,26 +7791,26 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H27" s="12" t="s">
-        <v>17</v>
+      <c r="B27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -6352,1530 +7865,6 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
-      <c r="A35" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-    </row>
-    <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="7"/>
-      <c r="B37" s="8"/>
-    </row>
-    <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="8"/>
-      <c r="B38" s="7"/>
-    </row>
-    <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="8"/>
-      <c r="B39" s="7"/>
-    </row>
-    <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="8"/>
-      <c r="B40" s="7"/>
-    </row>
-    <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="8"/>
-      <c r="B41" s="9"/>
-    </row>
-    <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A42" s="8"/>
-      <c r="B42" s="7"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:H42"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
-  <cols>
-    <col min="1" max="1" width="18.75" style="1" customWidth="1"/>
-    <col min="2" max="8" width="25.5625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A1" s="2"/>
-      <c r="B1" s="3">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" s="1" customFormat="1" ht="89" customHeight="1" spans="1:8">
-      <c r="A5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
-      <c r="A6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-    </row>
-    <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3">
-        <v>8</v>
-      </c>
-      <c r="C9" s="3">
-        <v>9</v>
-      </c>
-      <c r="D9" s="3">
-        <v>10</v>
-      </c>
-      <c r="E9" s="3">
-        <v>11</v>
-      </c>
-      <c r="F9" s="3">
-        <v>12</v>
-      </c>
-      <c r="G9" s="3">
-        <v>13</v>
-      </c>
-      <c r="H9" s="3">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A10" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A11" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A12" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" s="1" customFormat="1" ht="162" customHeight="1" spans="1:8">
-      <c r="A13" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A16" s="2"/>
-      <c r="B16" s="3">
-        <v>15</v>
-      </c>
-      <c r="C16" s="3">
-        <v>16</v>
-      </c>
-      <c r="D16" s="3">
-        <v>17</v>
-      </c>
-      <c r="E16" s="3">
-        <v>18</v>
-      </c>
-      <c r="F16" s="3">
-        <v>19</v>
-      </c>
-      <c r="G16" s="3">
-        <v>20</v>
-      </c>
-      <c r="H16" s="3">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A17" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A18" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-    </row>
-    <row r="19" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A19" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-    </row>
-    <row r="20" s="1" customFormat="1" ht="118" customHeight="1" spans="1:8">
-      <c r="A20" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A21" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-    </row>
-    <row r="23" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A23" s="2"/>
-      <c r="B23" s="3">
-        <v>22</v>
-      </c>
-      <c r="C23" s="3">
-        <v>23</v>
-      </c>
-      <c r="D23" s="6">
-        <v>24</v>
-      </c>
-      <c r="E23" s="6">
-        <v>25</v>
-      </c>
-      <c r="F23" s="6">
-        <v>26</v>
-      </c>
-      <c r="G23" s="6">
-        <v>27</v>
-      </c>
-      <c r="H23" s="6">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A24" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-    </row>
-    <row r="25" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A25" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-    </row>
-    <row r="26" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A26" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-    </row>
-    <row r="27" s="1" customFormat="1" ht="119" customHeight="1" spans="1:8">
-      <c r="A27" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A28" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-    </row>
-    <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
-      <c r="A30" s="2"/>
-      <c r="B30" s="6">
-        <v>29</v>
-      </c>
-      <c r="C30" s="6">
-        <v>30</v>
-      </c>
-      <c r="D30" s="6">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" s="1" customFormat="1" customHeight="1" spans="1:4">
-      <c r="A31" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-    </row>
-    <row r="32" s="1" customFormat="1" customHeight="1" spans="1:4">
-      <c r="A32" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-    </row>
-    <row r="33" s="1" customFormat="1" customHeight="1" spans="1:4">
-      <c r="A33" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-    </row>
-    <row r="34" s="1" customFormat="1" ht="134" customHeight="1" spans="1:4">
-      <c r="A34" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
-      <c r="A35" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-    </row>
-    <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="7"/>
-      <c r="B37" s="8"/>
-    </row>
-    <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="8"/>
-      <c r="B38" s="7"/>
-    </row>
-    <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="8"/>
-      <c r="B39" s="7"/>
-    </row>
-    <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="8"/>
-      <c r="B40" s="7"/>
-    </row>
-    <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="8"/>
-      <c r="B41" s="9"/>
-    </row>
-    <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A42" s="8"/>
-      <c r="B42" s="7"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:H42"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
-  <cols>
-    <col min="1" max="1" width="18.75" style="1" customWidth="1"/>
-    <col min="2" max="8" width="25.5625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A1" s="2"/>
-      <c r="B1" s="3">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" s="1" customFormat="1" ht="89" customHeight="1" spans="1:8">
-      <c r="A5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
-      <c r="A6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-    </row>
-    <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3">
-        <v>8</v>
-      </c>
-      <c r="C9" s="3">
-        <v>9</v>
-      </c>
-      <c r="D9" s="3">
-        <v>10</v>
-      </c>
-      <c r="E9" s="3">
-        <v>11</v>
-      </c>
-      <c r="F9" s="3">
-        <v>12</v>
-      </c>
-      <c r="G9" s="3">
-        <v>13</v>
-      </c>
-      <c r="H9" s="3">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A10" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A11" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A12" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" s="1" customFormat="1" ht="162" customHeight="1" spans="1:8">
-      <c r="A13" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A16" s="2"/>
-      <c r="B16" s="3">
-        <v>15</v>
-      </c>
-      <c r="C16" s="3">
-        <v>16</v>
-      </c>
-      <c r="D16" s="3">
-        <v>17</v>
-      </c>
-      <c r="E16" s="3">
-        <v>18</v>
-      </c>
-      <c r="F16" s="3">
-        <v>19</v>
-      </c>
-      <c r="G16" s="3">
-        <v>20</v>
-      </c>
-      <c r="H16" s="3">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A17" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A18" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-    </row>
-    <row r="19" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A19" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-    </row>
-    <row r="20" s="1" customFormat="1" ht="118" customHeight="1" spans="1:8">
-      <c r="A20" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A21" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-    </row>
-    <row r="23" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A23" s="2"/>
-      <c r="B23" s="3">
-        <v>22</v>
-      </c>
-      <c r="C23" s="3">
-        <v>23</v>
-      </c>
-      <c r="D23" s="6">
-        <v>24</v>
-      </c>
-      <c r="E23" s="6">
-        <v>25</v>
-      </c>
-      <c r="F23" s="6">
-        <v>26</v>
-      </c>
-      <c r="G23" s="6">
-        <v>27</v>
-      </c>
-      <c r="H23" s="6">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A24" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-    </row>
-    <row r="25" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A25" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-    </row>
-    <row r="26" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A26" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-    </row>
-    <row r="27" s="1" customFormat="1" ht="119" customHeight="1" spans="1:8">
-      <c r="A27" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A28" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-    </row>
-    <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
-      <c r="A30" s="2"/>
-      <c r="B30" s="6">
-        <v>29</v>
-      </c>
-      <c r="C30" s="6">
-        <v>30</v>
-      </c>
-      <c r="D30" s="6">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" s="1" customFormat="1" customHeight="1" spans="1:4">
-      <c r="A31" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-    </row>
-    <row r="32" s="1" customFormat="1" customHeight="1" spans="1:4">
-      <c r="A32" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-    </row>
-    <row r="33" s="1" customFormat="1" customHeight="1" spans="1:4">
-      <c r="A33" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-    </row>
-    <row r="34" s="1" customFormat="1" ht="134" customHeight="1" spans="1:4">
-      <c r="A34" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
-      <c r="A35" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-    </row>
-    <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="7"/>
-      <c r="B37" s="8"/>
-    </row>
-    <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="8"/>
-      <c r="B38" s="7"/>
-    </row>
-    <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="8"/>
-      <c r="B39" s="7"/>
-    </row>
-    <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="8"/>
-      <c r="B40" s="7"/>
-    </row>
-    <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="8"/>
-      <c r="B41" s="9"/>
-    </row>
-    <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A42" s="8"/>
-      <c r="B42" s="7"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:H42"/>
-  <sheetViews>
-    <sheetView topLeftCell="D28" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34:D34"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
-  <cols>
-    <col min="1" max="1" width="18.75" style="1" customWidth="1"/>
-    <col min="2" max="8" width="25.5625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A1" s="2"/>
-      <c r="B1" s="3">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" s="1" customFormat="1" ht="89" customHeight="1" spans="1:8">
-      <c r="A5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
-      <c r="A6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-    </row>
-    <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3">
-        <v>8</v>
-      </c>
-      <c r="C9" s="3">
-        <v>9</v>
-      </c>
-      <c r="D9" s="3">
-        <v>10</v>
-      </c>
-      <c r="E9" s="3">
-        <v>11</v>
-      </c>
-      <c r="F9" s="3">
-        <v>12</v>
-      </c>
-      <c r="G9" s="3">
-        <v>13</v>
-      </c>
-      <c r="H9" s="3">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A10" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A11" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A12" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" s="1" customFormat="1" ht="162" customHeight="1" spans="1:8">
-      <c r="A13" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A16" s="2"/>
-      <c r="B16" s="3">
-        <v>15</v>
-      </c>
-      <c r="C16" s="3">
-        <v>16</v>
-      </c>
-      <c r="D16" s="3">
-        <v>17</v>
-      </c>
-      <c r="E16" s="3">
-        <v>18</v>
-      </c>
-      <c r="F16" s="3">
-        <v>19</v>
-      </c>
-      <c r="G16" s="3">
-        <v>20</v>
-      </c>
-      <c r="H16" s="3">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A17" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A18" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-    </row>
-    <row r="19" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A19" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-    </row>
-    <row r="20" s="1" customFormat="1" ht="118" customHeight="1" spans="1:8">
-      <c r="A20" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A21" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-    </row>
-    <row r="23" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A23" s="2"/>
-      <c r="B23" s="3">
-        <v>22</v>
-      </c>
-      <c r="C23" s="3">
-        <v>23</v>
-      </c>
-      <c r="D23" s="6">
-        <v>24</v>
-      </c>
-      <c r="E23" s="6">
-        <v>25</v>
-      </c>
-      <c r="F23" s="6">
-        <v>26</v>
-      </c>
-      <c r="G23" s="6">
-        <v>27</v>
-      </c>
-      <c r="H23" s="6">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A24" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-    </row>
-    <row r="25" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A25" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-    </row>
-    <row r="26" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A26" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-    </row>
-    <row r="27" s="1" customFormat="1" ht="119" customHeight="1" spans="1:8">
-      <c r="A27" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
-      <c r="A28" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-    </row>
-    <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
-      <c r="A30" s="2"/>
-      <c r="B30" s="6">
-        <v>29</v>
-      </c>
-      <c r="C30" s="6">
-        <v>30</v>
-      </c>
-      <c r="D30" s="6">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" s="1" customFormat="1" customHeight="1" spans="1:4">
-      <c r="A31" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-    </row>
-    <row r="32" s="1" customFormat="1" customHeight="1" spans="1:4">
-      <c r="A32" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-    </row>
-    <row r="33" s="1" customFormat="1" customHeight="1" spans="1:4">
-      <c r="A33" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-    </row>
-    <row r="34" s="1" customFormat="1" ht="134" customHeight="1" spans="1:4">
-      <c r="A34" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="B34" s="5" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Tue May 16 09:11:49 CST 2023
</commit_message>
<xml_diff>
--- a/计划/2023学习计划.xlsx
+++ b/计划/2023学习计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16700" activeTab="10"/>
+    <workbookView windowHeight="16700" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -206,6 +206,44 @@
   </si>
   <si>
     <r>
+      <t>1音频/1视频/10技术书/1习题</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1音频/1视频/10技术书/1习题</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/1视频/10技术书/1习题</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <rPr>
         <strike/>
         <sz val="11"/>
@@ -228,11 +266,6 @@
 1音频/1视频/10技术书/1习题
 1音频/1视频/10技术书/1习题</t>
     </r>
-  </si>
-  <si>
-    <t>1音频/1视频/10技术书/1习题
-1音频/1视频/10技术书/1习题
-1音频/1视频/10技术书/1习题</t>
   </si>
   <si>
     <r>
@@ -275,9 +308,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
@@ -319,7 +352,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -327,29 +360,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -363,18 +373,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -386,8 +388,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -400,11 +411,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -432,25 +458,32 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -509,31 +542,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -545,13 +566,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -569,19 +590,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -593,55 +698,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -653,25 +710,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -683,13 +722,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -718,15 +751,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -738,6 +762,32 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -759,17 +809,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -781,22 +820,16 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -820,148 +853,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="35" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="34" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2348,8 +2381,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -2807,10 +2840,10 @@
         <v>22</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -2856,8 +2889,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="D28" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -2932,25 +2965,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -3042,25 +3075,25 @@
         <v>3</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3140,25 +3173,25 @@
         <v>3</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3238,25 +3271,25 @@
         <v>3</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3312,13 +3345,13 @@
         <v>3</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -8505,8 +8538,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -8694,21 +8727,21 @@
         <v>20</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="F13" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="G13" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="11" t="s">
         <v>21</v>
       </c>
     </row>
@@ -8788,25 +8821,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="G20" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="H20" s="5" t="s">
+      <c r="H20" s="11" t="s">
         <v>21</v>
       </c>
     </row>
@@ -8886,25 +8919,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="E27" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="F27" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="G27" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="H27" s="11" t="s">
         <v>21</v>
       </c>
     </row>
@@ -8960,13 +8993,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="11" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Mon Jul 31 20:46:43 CST 2023
</commit_message>
<xml_diff>
--- a/计划/2023学习计划.xlsx
+++ b/计划/2023学习计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13220" firstSheet="3" activeTab="14"/>
+    <workbookView windowHeight="16820" firstSheet="3" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="20">
   <si>
     <t>早餐</t>
   </si>
@@ -149,44 +149,6 @@
   </si>
   <si>
     <r>
-      <t>1音频/1视频/10技术书/1习题</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>20非技术书</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-1音频/1视频/10技术书/1习题</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
@@ -259,14 +221,6 @@
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -410,6 +364,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -771,152 +733,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -951,9 +913,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2296,8 +2255,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="C22" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -2695,8 +2654,8 @@
       <c r="G27" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H27" s="12" t="s">
-        <v>19</v>
+      <c r="H27" s="11" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -2751,14 +2710,14 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>20</v>
+      <c r="B34" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -2804,8 +2763,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -2879,26 +2838,26 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>20</v>
+      <c r="B5" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -2990,25 +2949,25 @@
         <v>3</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3088,25 +3047,25 @@
         <v>3</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3186,25 +3145,25 @@
         <v>3</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3260,13 +3219,13 @@
         <v>3</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -3388,25 +3347,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -3498,25 +3457,25 @@
         <v>3</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3596,25 +3555,25 @@
         <v>3</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3694,25 +3653,25 @@
         <v>3</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3768,13 +3727,13 @@
         <v>3</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -3896,25 +3855,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -4006,25 +3965,25 @@
         <v>3</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4104,25 +4063,25 @@
         <v>3</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4202,25 +4161,25 @@
         <v>3</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4276,13 +4235,13 @@
         <v>3</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -4329,7 +4288,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -4404,25 +4363,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -4514,16 +4473,16 @@
         <v>3</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>4</v>
@@ -5249,13 +5208,13 @@
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
-      <c r="F28" s="13" t="s">
+      <c r="F28" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G28" s="13" t="s">
+      <c r="G28" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="H28" s="13" t="s">
+      <c r="H28" s="12" t="s">
         <v>11</v>
       </c>
     </row>
@@ -5313,13 +5272,13 @@
       <c r="A35" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D35" s="13" t="s">
+      <c r="D35" s="12" t="s">
         <v>14</v>
       </c>
     </row>
@@ -5471,25 +5430,25 @@
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="12" t="s">
         <v>14</v>
       </c>
     </row>
@@ -5583,7 +5542,7 @@
       <c r="A14" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="12" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="2"/>
@@ -5591,7 +5550,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="13" t="s">
+      <c r="H14" s="12" t="s">
         <v>15</v>
       </c>
     </row>
@@ -5685,19 +5644,19 @@
       <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
-      <c r="G21" s="13" t="s">
+      <c r="G21" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H21" s="13" t="s">
+      <c r="H21" s="12" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5791,25 +5750,25 @@
       <c r="A28" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="D28" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E28" s="13" t="s">
+      <c r="E28" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F28" s="13" t="s">
+      <c r="F28" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G28" s="13" t="s">
+      <c r="G28" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H28" s="13" t="s">
+      <c r="H28" s="12" t="s">
         <v>14</v>
       </c>
     </row>
@@ -5961,25 +5920,25 @@
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="12" t="s">
         <v>14</v>
       </c>
     </row>
@@ -6073,25 +6032,25 @@
       <c r="A14" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="F14" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="G14" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="13" t="s">
+      <c r="H14" s="12" t="s">
         <v>14</v>
       </c>
     </row>
@@ -6185,25 +6144,25 @@
       <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="E21" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F21" s="13" t="s">
+      <c r="F21" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G21" s="13" t="s">
+      <c r="G21" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H21" s="13" t="s">
+      <c r="H21" s="12" t="s">
         <v>14</v>
       </c>
     </row>
@@ -6297,16 +6256,16 @@
       <c r="A28" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="D28" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E28" s="13" t="s">
+      <c r="E28" s="12" t="s">
         <v>14</v>
       </c>
       <c r="F28" s="2" t="s">
@@ -6631,7 +6590,7 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="12" t="s">
         <v>9</v>
       </c>
       <c r="E14" s="2"/>

</xml_diff>

<commit_message>
Fri Aug 11 23:26:46 CST 2023
</commit_message>
<xml_diff>
--- a/计划/2023学习计划.xlsx
+++ b/计划/2023学习计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16820" firstSheet="3" activeTab="14"/>
+    <workbookView windowHeight="16820" firstSheet="3" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="21">
   <si>
     <t>早餐</t>
   </si>
@@ -149,6 +149,44 @@
   </si>
   <si>
     <r>
+      <t>1音频/1视频/10技术书/1习题</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>20非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1音频/1视频/10技术书/1习题</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
@@ -221,6 +259,14 @@
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -364,14 +410,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -733,152 +771,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -913,6 +951,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1747,8 +1788,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -2763,8 +2804,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -2841,23 +2882,23 @@
       <c r="B5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>19</v>
+      <c r="C5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -2948,26 +2989,26 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3047,25 +3088,25 @@
         <v>3</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3145,25 +3186,25 @@
         <v>3</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3219,13 +3260,13 @@
         <v>3</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -3347,25 +3388,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -3457,25 +3498,25 @@
         <v>3</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3555,25 +3596,25 @@
         <v>3</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3653,25 +3694,25 @@
         <v>3</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3727,13 +3768,13 @@
         <v>3</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -3855,25 +3896,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -3965,25 +4006,25 @@
         <v>3</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4063,25 +4104,25 @@
         <v>3</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4161,25 +4202,25 @@
         <v>3</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4235,13 +4276,13 @@
         <v>3</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -4287,8 +4328,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -4363,25 +4404,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -4473,19 +4514,19 @@
         <v>3</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>4</v>
@@ -5208,13 +5249,13 @@
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
-      <c r="F28" s="12" t="s">
+      <c r="F28" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G28" s="12" t="s">
+      <c r="G28" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H28" s="12" t="s">
+      <c r="H28" s="13" t="s">
         <v>11</v>
       </c>
     </row>
@@ -5272,13 +5313,13 @@
       <c r="A35" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C35" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D35" s="12" t="s">
+      <c r="D35" s="13" t="s">
         <v>14</v>
       </c>
     </row>
@@ -5430,25 +5471,25 @@
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="13" t="s">
         <v>14</v>
       </c>
     </row>
@@ -5542,7 +5583,7 @@
       <c r="A14" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="2"/>
@@ -5550,7 +5591,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="12" t="s">
+      <c r="H14" s="13" t="s">
         <v>15</v>
       </c>
     </row>
@@ -5644,19 +5685,19 @@
       <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="13" t="s">
         <v>12</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
-      <c r="G21" s="12" t="s">
+      <c r="G21" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H21" s="12" t="s">
+      <c r="H21" s="13" t="s">
         <v>16</v>
       </c>
     </row>
@@ -5750,25 +5791,25 @@
       <c r="A28" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D28" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E28" s="12" t="s">
+      <c r="E28" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F28" s="12" t="s">
+      <c r="F28" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G28" s="12" t="s">
+      <c r="G28" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H28" s="12" t="s">
+      <c r="H28" s="13" t="s">
         <v>14</v>
       </c>
     </row>
@@ -5920,25 +5961,25 @@
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="13" t="s">
         <v>14</v>
       </c>
     </row>
@@ -6032,25 +6073,25 @@
       <c r="A14" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="G14" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="12" t="s">
+      <c r="H14" s="13" t="s">
         <v>14</v>
       </c>
     </row>
@@ -6144,25 +6185,25 @@
       <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="E21" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F21" s="12" t="s">
+      <c r="F21" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G21" s="12" t="s">
+      <c r="G21" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H21" s="12" t="s">
+      <c r="H21" s="13" t="s">
         <v>14</v>
       </c>
     </row>
@@ -6256,16 +6297,16 @@
       <c r="A28" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D28" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E28" s="12" t="s">
+      <c r="E28" s="13" t="s">
         <v>14</v>
       </c>
       <c r="F28" s="2" t="s">
@@ -6590,7 +6631,7 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="13" t="s">
         <v>9</v>
       </c>
       <c r="E14" s="2"/>

</xml_diff>

<commit_message>
Sun Nov  5 06:14:45 CST 2023
</commit_message>
<xml_diff>
--- a/计划/2023学习计划.xlsx
+++ b/计划/2023学习计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16820" firstSheet="3" activeTab="15"/>
+    <workbookView windowHeight="16220" firstSheet="3" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -151,14 +151,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>1音频/1视频/10技术书/1习题</t>
     </r>
     <r>
@@ -236,10 +228,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -288,8 +280,67 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -304,14 +355,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -326,21 +393,6 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -350,69 +402,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -470,13 +462,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -488,55 +534,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -554,25 +552,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -584,73 +636,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -675,21 +667,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -728,21 +705,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -768,6 +730,36 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -781,142 +773,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2814,8 +2806,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -3011,14 +3003,14 @@
       <c r="E13" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="12" t="s">
         <v>19</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4846,8 +4838,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -5130,25 +5122,25 @@
         <v>3</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5228,25 +5220,25 @@
         <v>3</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5302,13 +5294,13 @@
         <v>3</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -5354,8 +5346,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="$A1:$XFD1048576"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -5430,25 +5422,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -5540,25 +5532,25 @@
         <v>3</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5638,19 +5630,19 @@
         <v>3</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Wed Nov 15 01:15:12 CST 2023
</commit_message>
<xml_diff>
--- a/计划/2023学习计划.xlsx
+++ b/计划/2023学习计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="23420" firstSheet="3" activeTab="16"/>
+    <workbookView windowHeight="23420" firstSheet="3" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -24,13 +24,14 @@
     <sheet name="额外-2" sheetId="16" r:id="rId15"/>
     <sheet name="额外-3" sheetId="17" r:id="rId16"/>
     <sheet name="额外-4" sheetId="18" r:id="rId17"/>
+    <sheet name="额外-5" sheetId="19" r:id="rId18"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="21">
   <si>
     <t>早餐</t>
   </si>
@@ -2806,8 +2807,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -3107,8 +3108,8 @@
       <c r="G20" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="H20" s="5" t="s">
-        <v>20</v>
+      <c r="H20" s="12" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3187,23 +3188,23 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>20</v>
+      <c r="B27" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>19</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>20</v>
@@ -5346,8 +5347,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -5746,7 +5747,7 @@
         <v>20</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5802,13 +5803,13 @@
         <v>3</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -5845,6 +5846,514 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="18.75" style="1" customWidth="1"/>
+    <col min="2" max="8" width="25.5625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" s="1" customFormat="1" ht="89" customHeight="1" spans="1:8">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3">
+        <v>9</v>
+      </c>
+      <c r="D9" s="3">
+        <v>10</v>
+      </c>
+      <c r="E9" s="3">
+        <v>11</v>
+      </c>
+      <c r="F9" s="3">
+        <v>12</v>
+      </c>
+      <c r="G9" s="3">
+        <v>13</v>
+      </c>
+      <c r="H9" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" s="1" customFormat="1" ht="162" customHeight="1" spans="1:8">
+      <c r="A13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A16" s="2"/>
+      <c r="B16" s="3">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3">
+        <v>16</v>
+      </c>
+      <c r="D16" s="3">
+        <v>17</v>
+      </c>
+      <c r="E16" s="3">
+        <v>18</v>
+      </c>
+      <c r="F16" s="3">
+        <v>19</v>
+      </c>
+      <c r="G16" s="3">
+        <v>20</v>
+      </c>
+      <c r="H16" s="3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A18" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A19" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" s="1" customFormat="1" ht="118" customHeight="1" spans="1:8">
+      <c r="A20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="23" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A23" s="2"/>
+      <c r="B23" s="3">
+        <v>22</v>
+      </c>
+      <c r="C23" s="3">
+        <v>23</v>
+      </c>
+      <c r="D23" s="6">
+        <v>24</v>
+      </c>
+      <c r="E23" s="6">
+        <v>25</v>
+      </c>
+      <c r="F23" s="6">
+        <v>26</v>
+      </c>
+      <c r="G23" s="6">
+        <v>27</v>
+      </c>
+      <c r="H23" s="6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A25" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A26" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" s="1" customFormat="1" ht="119" customHeight="1" spans="1:8">
+      <c r="A27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A28" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A30" s="2"/>
+      <c r="B30" s="6">
+        <v>29</v>
+      </c>
+      <c r="C30" s="6">
+        <v>30</v>
+      </c>
+      <c r="D30" s="6">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A31" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A32" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A33" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" s="1" customFormat="1" ht="134" customHeight="1" spans="1:4">
+      <c r="A34" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A35" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A37" s="7"/>
+      <c r="B37" s="8"/>
+    </row>
+    <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A38" s="8"/>
+      <c r="B38" s="7"/>
+    </row>
+    <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A39" s="8"/>
+      <c r="B39" s="7"/>
+    </row>
+    <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A40" s="8"/>
+      <c r="B40" s="7"/>
+    </row>
+    <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
+      <c r="A41" s="8"/>
+      <c r="B41" s="9"/>
+    </row>
+    <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A42" s="8"/>
+      <c r="B42" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Wed Nov 15 10:27:33 CST 2023
</commit_message>
<xml_diff>
--- a/计划/2023学习计划.xlsx
+++ b/计划/2023学习计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="23420" firstSheet="3" activeTab="17"/>
+    <workbookView windowHeight="16220" firstSheet="3" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -2807,8 +2807,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -3206,8 +3206,8 @@
       <c r="G27" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="H27" s="5" t="s">
-        <v>20</v>
+      <c r="H27" s="12" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3262,11 +3262,11 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>20</v>
+      <c r="B34" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>19</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>20</v>
@@ -5855,7 +5855,7 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Wed Dec 13 22:03:58 CST 2023
</commit_message>
<xml_diff>
--- a/计划/2023学习计划.xlsx
+++ b/计划/2023学习计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13220" firstSheet="8" activeTab="17"/>
+    <workbookView windowHeight="24020" firstSheet="8" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -6023,7 +6023,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -6210,23 +6210,23 @@
       <c r="B13" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>23</v>
+      <c r="C13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -6305,11 +6305,11 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>23</v>
+      <c r="B20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Mon Dec 25 20:31:15 CST 2023
</commit_message>
<xml_diff>
--- a/计划/2023学习计划.xlsx
+++ b/计划/2023学习计划.xlsx
@@ -25,13 +25,14 @@
     <sheet name="额外-3" sheetId="17" r:id="rId16"/>
     <sheet name="额外-4" sheetId="18" r:id="rId17"/>
     <sheet name="额外-5" sheetId="19" r:id="rId18"/>
+    <sheet name="额外-6" sheetId="20" r:id="rId19"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="26">
   <si>
     <t>早餐</t>
   </si>
@@ -209,6 +210,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>1音视频/10技术书/复习1/1习题</t>
     </r>
     <r>
@@ -259,6 +268,52 @@
   <si>
     <r>
       <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1音视频/10技术书/复习1/1习题</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>20非技术书</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1音视频/10技术书/复习1/1习题</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -293,6 +348,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>20非技术书</t>
     </r>
     <r>
@@ -386,6 +449,11 @@
 20非技术书</t>
     </r>
   </si>
+  <si>
+    <t>20非技术书
+20非技术书
+20非技术书</t>
+  </si>
 </sst>
 </file>
 
@@ -393,9 +461,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -414,14 +482,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -431,13 +491,28 @@
       <strike/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -446,6 +521,20 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -460,10 +549,25 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -472,13 +576,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -497,8 +594,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -513,67 +640,8 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -614,19 +682,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="-0.5"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -644,7 +730,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -656,55 +742,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -722,7 +760,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -734,7 +778,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -746,7 +820,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -758,31 +844,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -794,19 +868,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -835,11 +903,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -848,7 +922,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -868,41 +942,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -932,153 +976,177 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1098,16 +1166,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1119,13 +1181,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1524,25 +1592,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1550,13 +1618,13 @@
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -1634,25 +1702,25 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1732,25 +1800,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1774,19 +1842,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="6">
         <v>24</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="6">
         <v>25</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="6">
         <v>26</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="6">
         <v>27</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="6">
         <v>28</v>
       </c>
     </row>
@@ -1830,25 +1898,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="E27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="F27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="G27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H27" s="6" t="s">
+      <c r="H27" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1866,13 +1934,13 @@
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A30" s="2"/>
-      <c r="B30" s="8">
+      <c r="B30" s="6">
         <v>29</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="6">
         <v>30</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="6">
         <v>31</v>
       </c>
     </row>
@@ -1904,13 +1972,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1923,28 +1991,28 @@
       <c r="D35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="9"/>
-      <c r="B37" s="10"/>
+      <c r="A37" s="7"/>
+      <c r="B37" s="8"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="10"/>
-      <c r="B38" s="9"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="7"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="10"/>
-      <c r="B39" s="9"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="7"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="10"/>
-      <c r="B40" s="9"/>
+      <c r="A40" s="8"/>
+      <c r="B40" s="7"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="10"/>
-      <c r="B41" s="11"/>
+      <c r="A41" s="8"/>
+      <c r="B41" s="9"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A42" s="10"/>
-      <c r="B42" s="9"/>
+      <c r="A42" s="8"/>
+      <c r="B42" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -2058,13 +2126,13 @@
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -2282,19 +2350,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="6">
         <v>24</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="6">
         <v>25</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="6">
         <v>26</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="6">
         <v>27</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="6">
         <v>28</v>
       </c>
     </row>
@@ -2374,13 +2442,13 @@
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A30" s="2"/>
-      <c r="B30" s="8">
+      <c r="B30" s="6">
         <v>29</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="6">
         <v>30</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="6">
         <v>31</v>
       </c>
     </row>
@@ -2431,28 +2499,28 @@
       <c r="D35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="9"/>
-      <c r="B37" s="10"/>
+      <c r="A37" s="7"/>
+      <c r="B37" s="8"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="10"/>
-      <c r="B38" s="9"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="7"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="10"/>
-      <c r="B39" s="9"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="7"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="10"/>
-      <c r="B40" s="9"/>
+      <c r="A40" s="8"/>
+      <c r="B40" s="7"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="10"/>
-      <c r="B41" s="11"/>
+      <c r="A41" s="8"/>
+      <c r="B41" s="9"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A42" s="10"/>
-      <c r="B42" s="9"/>
+      <c r="A42" s="8"/>
+      <c r="B42" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -2566,13 +2634,13 @@
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -2790,19 +2858,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="6">
         <v>24</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="6">
         <v>25</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="6">
         <v>26</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="6">
         <v>27</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="6">
         <v>28</v>
       </c>
     </row>
@@ -2882,13 +2950,13 @@
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A30" s="2"/>
-      <c r="B30" s="8">
+      <c r="B30" s="6">
         <v>29</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="6">
         <v>30</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="6">
         <v>31</v>
       </c>
     </row>
@@ -2939,28 +3007,28 @@
       <c r="D35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="9"/>
-      <c r="B37" s="10"/>
+      <c r="A37" s="7"/>
+      <c r="B37" s="8"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="10"/>
-      <c r="B38" s="9"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="7"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="10"/>
-      <c r="B39" s="9"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="7"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="10"/>
-      <c r="B40" s="9"/>
+      <c r="A40" s="8"/>
+      <c r="B40" s="7"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="10"/>
-      <c r="B41" s="11"/>
+      <c r="A41" s="8"/>
+      <c r="B41" s="9"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A42" s="10"/>
-      <c r="B42" s="9"/>
+      <c r="A42" s="8"/>
+      <c r="B42" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -3074,13 +3142,13 @@
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -3259,22 +3327,22 @@
       <c r="B20" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="G20" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="H20" s="5" t="s">
+      <c r="H20" s="11" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3298,19 +3366,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="6">
         <v>24</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="6">
         <v>25</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="6">
         <v>26</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="6">
         <v>27</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="6">
         <v>28</v>
       </c>
     </row>
@@ -3354,25 +3422,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="E27" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="F27" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="G27" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="H27" s="11" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3390,13 +3458,13 @@
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A30" s="2"/>
-      <c r="B30" s="8">
+      <c r="B30" s="6">
         <v>29</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="6">
         <v>30</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="6">
         <v>31</v>
       </c>
     </row>
@@ -3428,13 +3496,13 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="11" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3447,28 +3515,28 @@
       <c r="D35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="9"/>
-      <c r="B37" s="10"/>
+      <c r="A37" s="7"/>
+      <c r="B37" s="8"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="10"/>
-      <c r="B38" s="9"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="7"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="10"/>
-      <c r="B39" s="9"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="7"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="10"/>
-      <c r="B40" s="9"/>
+      <c r="A40" s="8"/>
+      <c r="B40" s="7"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="10"/>
-      <c r="B41" s="11"/>
+      <c r="A41" s="8"/>
+      <c r="B41" s="9"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A42" s="10"/>
-      <c r="B42" s="9"/>
+      <c r="A42" s="8"/>
+      <c r="B42" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -3481,8 +3549,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -3557,25 +3625,25 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="G5" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="12" t="s">
         <v>21</v>
       </c>
     </row>
@@ -3583,13 +3651,13 @@
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -3667,26 +3735,26 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="6" t="s">
-        <v>21</v>
+      <c r="H13" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3765,26 +3833,26 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>21</v>
+      <c r="B20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3807,19 +3875,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="6">
         <v>24</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="6">
         <v>25</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="6">
         <v>26</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="6">
         <v>27</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="6">
         <v>28</v>
       </c>
     </row>
@@ -3863,26 +3931,26 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>21</v>
+      <c r="B27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -3899,13 +3967,13 @@
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A30" s="2"/>
-      <c r="B30" s="8">
+      <c r="B30" s="6">
         <v>29</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="6">
         <v>30</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="6">
         <v>31</v>
       </c>
     </row>
@@ -3937,14 +4005,14 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>21</v>
+      <c r="B34" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -3956,28 +4024,28 @@
       <c r="D35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="9"/>
-      <c r="B37" s="10"/>
+      <c r="A37" s="7"/>
+      <c r="B37" s="8"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="10"/>
-      <c r="B38" s="9"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="7"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="10"/>
-      <c r="B39" s="9"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="7"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="10"/>
-      <c r="B40" s="9"/>
+      <c r="A40" s="8"/>
+      <c r="B40" s="7"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="10"/>
-      <c r="B41" s="11"/>
+      <c r="A41" s="8"/>
+      <c r="B41" s="9"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A42" s="10"/>
-      <c r="B42" s="9"/>
+      <c r="A42" s="8"/>
+      <c r="B42" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -4065,39 +4133,39 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>21</v>
+      <c r="B5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -4175,26 +4243,26 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>21</v>
+      <c r="B13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4273,26 +4341,26 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>21</v>
+      <c r="B20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4315,19 +4383,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="6">
         <v>24</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="6">
         <v>25</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="6">
         <v>26</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="6">
         <v>27</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="6">
         <v>28</v>
       </c>
     </row>
@@ -4371,26 +4439,26 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>21</v>
+      <c r="B27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4407,13 +4475,13 @@
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A30" s="2"/>
-      <c r="B30" s="8">
+      <c r="B30" s="6">
         <v>29</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="6">
         <v>30</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="6">
         <v>31</v>
       </c>
     </row>
@@ -4445,14 +4513,14 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>21</v>
+      <c r="B34" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -4464,28 +4532,28 @@
       <c r="D35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="9"/>
-      <c r="B37" s="10"/>
+      <c r="A37" s="7"/>
+      <c r="B37" s="8"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="10"/>
-      <c r="B38" s="9"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="7"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="10"/>
-      <c r="B39" s="9"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="7"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="10"/>
-      <c r="B40" s="9"/>
+      <c r="A40" s="8"/>
+      <c r="B40" s="7"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="10"/>
-      <c r="B41" s="11"/>
+      <c r="A41" s="8"/>
+      <c r="B41" s="9"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A42" s="10"/>
-      <c r="B42" s="9"/>
+      <c r="A42" s="8"/>
+      <c r="B42" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4573,39 +4641,39 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>21</v>
+      <c r="B5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -4683,26 +4751,26 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>21</v>
+      <c r="B13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4781,26 +4849,26 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>21</v>
+      <c r="B20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4823,19 +4891,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="6">
         <v>24</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="6">
         <v>25</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="6">
         <v>26</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="6">
         <v>27</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="6">
         <v>28</v>
       </c>
     </row>
@@ -4879,26 +4947,26 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>21</v>
+      <c r="B27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -4915,13 +4983,13 @@
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A30" s="2"/>
-      <c r="B30" s="8">
+      <c r="B30" s="6">
         <v>29</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="6">
         <v>30</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="6">
         <v>31</v>
       </c>
     </row>
@@ -4953,14 +5021,14 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>21</v>
+      <c r="B34" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -4972,28 +5040,28 @@
       <c r="D35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="9"/>
-      <c r="B37" s="10"/>
+      <c r="A37" s="7"/>
+      <c r="B37" s="8"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="10"/>
-      <c r="B38" s="9"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="7"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="10"/>
-      <c r="B39" s="9"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="7"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="10"/>
-      <c r="B40" s="9"/>
+      <c r="A40" s="8"/>
+      <c r="B40" s="7"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="10"/>
-      <c r="B41" s="11"/>
+      <c r="A41" s="8"/>
+      <c r="B41" s="9"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A42" s="10"/>
-      <c r="B42" s="9"/>
+      <c r="A42" s="8"/>
+      <c r="B42" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -5081,39 +5149,39 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>21</v>
+      <c r="B5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -5191,26 +5259,26 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>21</v>
+      <c r="B13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5289,26 +5357,26 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>21</v>
+      <c r="B20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5331,19 +5399,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="6">
         <v>24</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="6">
         <v>25</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="6">
         <v>26</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="6">
         <v>27</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="6">
         <v>28</v>
       </c>
     </row>
@@ -5387,26 +5455,26 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>21</v>
+      <c r="B27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5423,13 +5491,13 @@
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A30" s="2"/>
-      <c r="B30" s="8">
+      <c r="B30" s="6">
         <v>29</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="6">
         <v>30</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="6">
         <v>31</v>
       </c>
     </row>
@@ -5461,14 +5529,14 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>21</v>
+      <c r="B34" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -5480,28 +5548,28 @@
       <c r="D35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="9"/>
-      <c r="B37" s="10"/>
+      <c r="A37" s="7"/>
+      <c r="B37" s="8"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="10"/>
-      <c r="B38" s="9"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="7"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="10"/>
-      <c r="B39" s="9"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="7"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="10"/>
-      <c r="B40" s="9"/>
+      <c r="A40" s="8"/>
+      <c r="B40" s="7"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="10"/>
-      <c r="B41" s="11"/>
+      <c r="A41" s="8"/>
+      <c r="B41" s="9"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A42" s="10"/>
-      <c r="B42" s="9"/>
+      <c r="A42" s="8"/>
+      <c r="B42" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -5589,39 +5657,39 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>21</v>
+      <c r="B5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -5699,26 +5767,26 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>21</v>
+      <c r="B13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5797,26 +5865,26 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>21</v>
+      <c r="B20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5839,19 +5907,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="6">
         <v>24</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="6">
         <v>25</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="6">
         <v>26</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="6">
         <v>27</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="6">
         <v>28</v>
       </c>
     </row>
@@ -5895,26 +5963,26 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>21</v>
+      <c r="B27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -5931,13 +5999,13 @@
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A30" s="2"/>
-      <c r="B30" s="8">
+      <c r="B30" s="6">
         <v>29</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="6">
         <v>30</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="6">
         <v>31</v>
       </c>
     </row>
@@ -5969,14 +6037,14 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>21</v>
+      <c r="B34" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -5988,28 +6056,28 @@
       <c r="D35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="9"/>
-      <c r="B37" s="10"/>
+      <c r="A37" s="7"/>
+      <c r="B37" s="8"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="10"/>
-      <c r="B38" s="9"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="7"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="10"/>
-      <c r="B39" s="9"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="7"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="10"/>
-      <c r="B40" s="9"/>
+      <c r="A40" s="8"/>
+      <c r="B40" s="7"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="10"/>
-      <c r="B41" s="11"/>
+      <c r="A41" s="8"/>
+      <c r="B41" s="9"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A42" s="10"/>
-      <c r="B42" s="9"/>
+      <c r="A42" s="8"/>
+      <c r="B42" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -6022,8 +6090,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -6097,39 +6165,39 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>22</v>
+      <c r="B5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -6207,26 +6275,26 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>22</v>
+      <c r="B13" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -6305,25 +6373,25 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="7" t="s">
+      <c r="B20" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="C20" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="D20" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="E20" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="H20" s="7" t="s">
+      <c r="F20" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20" s="11" t="s">
         <v>23</v>
       </c>
     </row>
@@ -6347,19 +6415,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="6">
         <v>24</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="6">
         <v>25</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="6">
         <v>26</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="6">
         <v>27</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="6">
         <v>28</v>
       </c>
     </row>
@@ -6403,25 +6471,25 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="F27" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="G27" s="7" t="s">
+      <c r="G27" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="H27" s="7" t="s">
+      <c r="H27" s="11" t="s">
         <v>23</v>
       </c>
     </row>
@@ -6439,13 +6507,13 @@
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A30" s="2"/>
-      <c r="B30" s="8">
+      <c r="B30" s="6">
         <v>29</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="6">
         <v>30</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="6">
         <v>31</v>
       </c>
     </row>
@@ -6477,14 +6545,14 @@
       <c r="A34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>23</v>
+      <c r="B34" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
@@ -6496,28 +6564,536 @@
       <c r="D35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="9"/>
-      <c r="B37" s="10"/>
+      <c r="A37" s="7"/>
+      <c r="B37" s="8"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="10"/>
-      <c r="B38" s="9"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="7"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="10"/>
-      <c r="B39" s="9"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="7"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="10"/>
-      <c r="B40" s="9"/>
+      <c r="A40" s="8"/>
+      <c r="B40" s="7"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="10"/>
-      <c r="B41" s="11"/>
+      <c r="A41" s="8"/>
+      <c r="B41" s="9"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A42" s="10"/>
-      <c r="B42" s="9"/>
+      <c r="A42" s="8"/>
+      <c r="B42" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="18.75" style="1" customWidth="1"/>
+    <col min="2" max="8" width="25.5625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" s="1" customFormat="1" ht="89" customHeight="1" spans="1:8">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="9" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3">
+        <v>9</v>
+      </c>
+      <c r="D9" s="3">
+        <v>10</v>
+      </c>
+      <c r="E9" s="3">
+        <v>11</v>
+      </c>
+      <c r="F9" s="3">
+        <v>12</v>
+      </c>
+      <c r="G9" s="3">
+        <v>13</v>
+      </c>
+      <c r="H9" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" s="1" customFormat="1" ht="162" customHeight="1" spans="1:8">
+      <c r="A13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A16" s="2"/>
+      <c r="B16" s="3">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3">
+        <v>16</v>
+      </c>
+      <c r="D16" s="3">
+        <v>17</v>
+      </c>
+      <c r="E16" s="3">
+        <v>18</v>
+      </c>
+      <c r="F16" s="3">
+        <v>19</v>
+      </c>
+      <c r="G16" s="3">
+        <v>20</v>
+      </c>
+      <c r="H16" s="3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A18" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A19" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" s="1" customFormat="1" ht="118" customHeight="1" spans="1:8">
+      <c r="A20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="23" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A23" s="2"/>
+      <c r="B23" s="3">
+        <v>22</v>
+      </c>
+      <c r="C23" s="3">
+        <v>23</v>
+      </c>
+      <c r="D23" s="6">
+        <v>24</v>
+      </c>
+      <c r="E23" s="6">
+        <v>25</v>
+      </c>
+      <c r="F23" s="6">
+        <v>26</v>
+      </c>
+      <c r="G23" s="6">
+        <v>27</v>
+      </c>
+      <c r="H23" s="6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A25" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A26" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" s="1" customFormat="1" ht="119" customHeight="1" spans="1:8">
+      <c r="A27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A28" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A30" s="2"/>
+      <c r="B30" s="6">
+        <v>29</v>
+      </c>
+      <c r="C30" s="6">
+        <v>30</v>
+      </c>
+      <c r="D30" s="6">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A31" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A32" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A33" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" s="1" customFormat="1" ht="134" customHeight="1" spans="1:4">
+      <c r="A34" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" s="1" customFormat="1" customHeight="1" spans="1:4">
+      <c r="A35" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A37" s="7"/>
+      <c r="B37" s="8"/>
+    </row>
+    <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A38" s="8"/>
+      <c r="B38" s="7"/>
+    </row>
+    <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A39" s="8"/>
+      <c r="B39" s="7"/>
+    </row>
+    <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A40" s="8"/>
+      <c r="B40" s="7"/>
+    </row>
+    <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
+      <c r="A41" s="8"/>
+      <c r="B41" s="9"/>
+    </row>
+    <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
+      <c r="A42" s="8"/>
+      <c r="B42" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6631,13 +7207,13 @@
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -6857,19 +7433,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="6">
         <v>24</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="6">
         <v>25</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="6">
         <v>26</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="6">
         <v>27</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="6">
         <v>28</v>
       </c>
     </row>
@@ -6955,13 +7531,13 @@
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A30" s="2"/>
-      <c r="B30" s="8">
+      <c r="B30" s="6">
         <v>29</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="6">
         <v>30</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="6">
         <v>31</v>
       </c>
     </row>
@@ -7018,28 +7594,28 @@
       </c>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="9"/>
-      <c r="B37" s="10"/>
+      <c r="A37" s="7"/>
+      <c r="B37" s="8"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="10"/>
-      <c r="B38" s="9"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="7"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="10"/>
-      <c r="B39" s="9"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="7"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="10"/>
-      <c r="B40" s="9"/>
+      <c r="A40" s="8"/>
+      <c r="B40" s="7"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="10"/>
-      <c r="B41" s="11"/>
+      <c r="A41" s="8"/>
+      <c r="B41" s="9"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A42" s="10"/>
-      <c r="B42" s="9"/>
+      <c r="A42" s="8"/>
+      <c r="B42" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -7153,13 +7729,13 @@
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -7403,19 +7979,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="6">
         <v>24</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="6">
         <v>25</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="6">
         <v>26</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="6">
         <v>27</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="6">
         <v>28</v>
       </c>
     </row>
@@ -7508,28 +8084,28 @@
       </c>
     </row>
     <row r="31" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A31" s="9"/>
-      <c r="B31" s="10"/>
+      <c r="A31" s="7"/>
+      <c r="B31" s="8"/>
     </row>
     <row r="32" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A32" s="10"/>
-      <c r="B32" s="9"/>
+      <c r="A32" s="8"/>
+      <c r="B32" s="7"/>
     </row>
     <row r="33" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A33" s="10"/>
-      <c r="B33" s="9"/>
+      <c r="A33" s="8"/>
+      <c r="B33" s="7"/>
     </row>
     <row r="34" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A34" s="10"/>
-      <c r="B34" s="9"/>
+      <c r="A34" s="8"/>
+      <c r="B34" s="7"/>
     </row>
     <row r="35" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A35" s="10"/>
-      <c r="B35" s="11"/>
+      <c r="A35" s="8"/>
+      <c r="B35" s="9"/>
     </row>
     <row r="36" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A36" s="10"/>
-      <c r="B36" s="9"/>
+      <c r="A36" s="8"/>
+      <c r="B36" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -7643,13 +8219,13 @@
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -7909,19 +8485,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="6">
         <v>24</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="6">
         <v>25</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="6">
         <v>26</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="6">
         <v>27</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="6">
         <v>28</v>
       </c>
     </row>
@@ -8015,13 +8591,13 @@
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A30" s="2"/>
-      <c r="B30" s="8">
+      <c r="B30" s="6">
         <v>29</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="6">
         <v>30</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="6">
         <v>31</v>
       </c>
     </row>
@@ -8078,28 +8654,28 @@
       </c>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="9"/>
-      <c r="B37" s="10"/>
+      <c r="A37" s="7"/>
+      <c r="B37" s="8"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="10"/>
-      <c r="B38" s="9"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="7"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="10"/>
-      <c r="B39" s="9"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="7"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="10"/>
-      <c r="B40" s="9"/>
+      <c r="A40" s="8"/>
+      <c r="B40" s="7"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="10"/>
-      <c r="B41" s="11"/>
+      <c r="A41" s="8"/>
+      <c r="B41" s="9"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A42" s="10"/>
-      <c r="B42" s="9"/>
+      <c r="A42" s="8"/>
+      <c r="B42" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -8213,13 +8789,13 @@
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -8439,19 +9015,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="6">
         <v>24</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="6">
         <v>25</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="6">
         <v>26</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="6">
         <v>27</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="6">
         <v>28</v>
       </c>
     </row>
@@ -8531,13 +9107,13 @@
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A30" s="2"/>
-      <c r="B30" s="8">
+      <c r="B30" s="6">
         <v>29</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="6">
         <v>30</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="6">
         <v>31</v>
       </c>
     </row>
@@ -8588,28 +9164,28 @@
       <c r="D35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="9"/>
-      <c r="B37" s="10"/>
+      <c r="A37" s="7"/>
+      <c r="B37" s="8"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="10"/>
-      <c r="B38" s="9"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="7"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="10"/>
-      <c r="B39" s="9"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="7"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="10"/>
-      <c r="B40" s="9"/>
+      <c r="A40" s="8"/>
+      <c r="B40" s="7"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="10"/>
-      <c r="B41" s="11"/>
+      <c r="A41" s="8"/>
+      <c r="B41" s="9"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A42" s="10"/>
-      <c r="B42" s="9"/>
+      <c r="A42" s="8"/>
+      <c r="B42" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -8724,13 +9300,13 @@
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -8948,19 +9524,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="6">
         <v>24</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="6">
         <v>25</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="6">
         <v>26</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="6">
         <v>27</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="6">
         <v>28</v>
       </c>
     </row>
@@ -9040,13 +9616,13 @@
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A30" s="2"/>
-      <c r="B30" s="8">
+      <c r="B30" s="6">
         <v>29</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="6">
         <v>30</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="6">
         <v>31</v>
       </c>
     </row>
@@ -9097,28 +9673,28 @@
       <c r="D35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="9"/>
-      <c r="B37" s="10"/>
+      <c r="A37" s="7"/>
+      <c r="B37" s="8"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="10"/>
-      <c r="B38" s="9"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="7"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="10"/>
-      <c r="B39" s="9"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="7"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="10"/>
-      <c r="B40" s="9"/>
+      <c r="A40" s="8"/>
+      <c r="B40" s="7"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="10"/>
-      <c r="B41" s="11"/>
+      <c r="A41" s="8"/>
+      <c r="B41" s="9"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A42" s="10"/>
-      <c r="B42" s="9"/>
+      <c r="A42" s="8"/>
+      <c r="B42" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -9232,13 +9808,13 @@
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -9456,19 +10032,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="6">
         <v>24</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="6">
         <v>25</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="6">
         <v>26</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="6">
         <v>27</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="6">
         <v>28</v>
       </c>
     </row>
@@ -9548,13 +10124,13 @@
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A30" s="2"/>
-      <c r="B30" s="8">
+      <c r="B30" s="6">
         <v>29</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="6">
         <v>30</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="6">
         <v>31</v>
       </c>
     </row>
@@ -9605,28 +10181,28 @@
       <c r="D35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="9"/>
-      <c r="B37" s="10"/>
+      <c r="A37" s="7"/>
+      <c r="B37" s="8"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="10"/>
-      <c r="B38" s="9"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="7"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="10"/>
-      <c r="B39" s="9"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="7"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="10"/>
-      <c r="B40" s="9"/>
+      <c r="A40" s="8"/>
+      <c r="B40" s="7"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="10"/>
-      <c r="B41" s="11"/>
+      <c r="A41" s="8"/>
+      <c r="B41" s="9"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A42" s="10"/>
-      <c r="B42" s="9"/>
+      <c r="A42" s="8"/>
+      <c r="B42" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -9740,13 +10316,13 @@
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -9964,19 +10540,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="6">
         <v>24</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="6">
         <v>25</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="6">
         <v>26</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="6">
         <v>27</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="6">
         <v>28</v>
       </c>
     </row>
@@ -10056,13 +10632,13 @@
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A30" s="2"/>
-      <c r="B30" s="8">
+      <c r="B30" s="6">
         <v>29</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="6">
         <v>30</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="6">
         <v>31</v>
       </c>
     </row>
@@ -10113,28 +10689,28 @@
       <c r="D35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="9"/>
-      <c r="B37" s="10"/>
+      <c r="A37" s="7"/>
+      <c r="B37" s="8"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="10"/>
-      <c r="B38" s="9"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="7"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="10"/>
-      <c r="B39" s="9"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="7"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="10"/>
-      <c r="B40" s="9"/>
+      <c r="A40" s="8"/>
+      <c r="B40" s="7"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="10"/>
-      <c r="B41" s="11"/>
+      <c r="A41" s="8"/>
+      <c r="B41" s="9"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A42" s="10"/>
-      <c r="B42" s="9"/>
+      <c r="A42" s="8"/>
+      <c r="B42" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -10248,13 +10824,13 @@
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:8">
       <c r="A7" s="4" t="s">
@@ -10472,19 +11048,19 @@
       <c r="C23" s="3">
         <v>23</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="6">
         <v>24</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="6">
         <v>25</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="6">
         <v>26</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="6">
         <v>27</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="6">
         <v>28</v>
       </c>
     </row>
@@ -10564,13 +11140,13 @@
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="1:4">
       <c r="A30" s="2"/>
-      <c r="B30" s="8">
+      <c r="B30" s="6">
         <v>29</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="6">
         <v>30</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="6">
         <v>31</v>
       </c>
     </row>
@@ -10621,28 +11197,28 @@
       <c r="D35" s="2"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A37" s="9"/>
-      <c r="B37" s="10"/>
+      <c r="A37" s="7"/>
+      <c r="B37" s="8"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A38" s="10"/>
-      <c r="B38" s="9"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="7"/>
     </row>
     <row r="39" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A39" s="10"/>
-      <c r="B39" s="9"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="7"/>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A40" s="10"/>
-      <c r="B40" s="9"/>
+      <c r="A40" s="8"/>
+      <c r="B40" s="7"/>
     </row>
     <row r="41" s="1" customFormat="1" ht="87" customHeight="1" spans="1:2">
-      <c r="A41" s="10"/>
-      <c r="B41" s="11"/>
+      <c r="A41" s="8"/>
+      <c r="B41" s="9"/>
     </row>
     <row r="42" s="1" customFormat="1" customHeight="1" spans="1:2">
-      <c r="A42" s="10"/>
-      <c r="B42" s="9"/>
+      <c r="A42" s="8"/>
+      <c r="B42" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>

</xml_diff>

<commit_message>
Sat Mar 23 19:29:39 CST 2024
</commit_message>
<xml_diff>
--- a/计划/2023学习计划.xlsx
+++ b/计划/2023学习计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16640" firstSheet="3" activeTab="18"/>
+    <workbookView windowHeight="23840" firstSheet="3" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -3528,8 +3528,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -3812,20 +3812,20 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>21</v>
+      <c r="B20" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>21</v>
@@ -6577,8 +6577,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -6667,11 +6667,11 @@
       <c r="F5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>25</v>
+      <c r="G5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="44" customHeight="1" spans="1:8">
@@ -6762,26 +6762,26 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>25</v>
+      <c r="B13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" customHeight="1" spans="1:8">

</xml_diff>

<commit_message>
Mon Mar 25 09:43:30 CST 2024
</commit_message>
<xml_diff>
--- a/计划/2023学习计划.xlsx
+++ b/计划/2023学习计划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="23840" firstSheet="3" activeTab="18"/>
+    <workbookView windowHeight="16640" firstSheet="3" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -6577,8 +6577,8 @@
   <sheetPr/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="40" customHeight="1" outlineLevelCol="7"/>
@@ -6860,26 +6860,26 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>25</v>
+      <c r="B20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:8">
@@ -6958,11 +6958,11 @@
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>25</v>
+      <c r="B27" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>25</v>

</xml_diff>